<commit_message>
item code accesories selected
</commit_message>
<xml_diff>
--- a/Resources/2-Datastore.xlsx
+++ b/Resources/2-Datastore.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="90" windowWidth="20580" windowHeight="11640" activeTab="2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>Customer</t>
   </si>
@@ -756,7 +756,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,13 +817,11 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F3" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F4" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="F4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added few images and steps related to remains to scirpt #2
</commit_message>
<xml_diff>
--- a/Resources/2-Datastore.xlsx
+++ b/Resources/2-Datastore.xlsx
@@ -126,9 +126,6 @@
     <t>Username</t>
   </si>
   <si>
-    <t>password</t>
-  </si>
-  <si>
     <t>customerNumber</t>
   </si>
   <si>
@@ -160,6 +157,9 @@
   </si>
   <si>
     <t>TB7SX6CC</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
@@ -756,7 +756,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="D3" sqref="D3:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,42 +774,42 @@
         <v>35</v>
       </c>
       <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
         <v>36</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>37</v>
-      </c>
-      <c r="D1" t="s">
-        <v>38</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
         <v>42</v>
       </c>
-      <c r="B2" t="s">
-        <v>43</v>
-      </c>
       <c r="C2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="D2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -817,7 +817,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>